<commit_message>
Timings file output and aerofoil wind tunnel config added for TIANHE2 cases
</commit_message>
<xml_diff>
--- a/LatBo/tools/ParabolicProfiles.xlsx
+++ b/LatBo/tools/ParabolicProfiles.xlsx
@@ -62,15 +62,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,15 +84,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,318 +206,624 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$50</c:f>
+              <c:f>Sheet1!$B:$B</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="1048576"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>-1.2307371928363064E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.03</c:v>
+                  <c:v>1.218242399000431E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>3.6172428154935465E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>5.9662640566430598E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0000000000000011E-2</c:v>
+                  <c:v>8.265306122448985E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11000000000000001</c:v>
+                  <c:v>1.0514369012911289E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13</c:v>
+                  <c:v>1.2713452728030003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.15</c:v>
+                  <c:v>1.4862557267805082E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16999999999999998</c:v>
+                  <c:v>1.696168263223656E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18999999999999997</c:v>
+                  <c:v>1.9010828821324457E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20999999999999996</c:v>
+                  <c:v>2.1009995835068716E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22999999999999995</c:v>
+                  <c:v>2.2959183673469389E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24999999999999994</c:v>
+                  <c:v>2.4858392336526453E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26999999999999996</c:v>
+                  <c:v>2.6707621824239906E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>2.8506872136609754E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.31</c:v>
+                  <c:v>3.0256143273635992E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.33</c:v>
+                  <c:v>3.195543523531863E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.35000000000000003</c:v>
+                  <c:v>3.3604748021657659E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.37000000000000005</c:v>
+                  <c:v>3.5204081632653074E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.39000000000000007</c:v>
+                  <c:v>3.6753436068304883E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.41000000000000009</c:v>
+                  <c:v>3.8252811328613086E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.4300000000000001</c:v>
+                  <c:v>3.9702207413577696E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.45000000000000012</c:v>
+                  <c:v>4.1101624323198679E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.47000000000000014</c:v>
+                  <c:v>4.245106205747607E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.49000000000000016</c:v>
+                  <c:v>4.3750520616409848E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.51000000000000012</c:v>
+                  <c:v>4.5000000000000012E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.53000000000000014</c:v>
+                  <c:v>4.6199500208246577E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.55000000000000016</c:v>
+                  <c:v>4.7349021241149536E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.57000000000000017</c:v>
+                  <c:v>4.8448563098708888E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.59000000000000019</c:v>
+                  <c:v>4.9498125780924634E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.61000000000000021</c:v>
+                  <c:v>5.049770928779676E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.63000000000000023</c:v>
+                  <c:v>5.1447313619325294E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.65000000000000024</c:v>
+                  <c:v>5.2346938775510214E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.67000000000000026</c:v>
+                  <c:v>5.3196584756351535E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.69000000000000028</c:v>
+                  <c:v>5.3996251561849243E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.7100000000000003</c:v>
+                  <c:v>5.4745939192003344E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.73000000000000032</c:v>
+                  <c:v>5.5445647646813839E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.75000000000000033</c:v>
+                  <c:v>5.6095376926280728E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.77000000000000035</c:v>
+                  <c:v>5.6695127030404011E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.79000000000000037</c:v>
+                  <c:v>5.7244897959183687E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.81000000000000039</c:v>
+                  <c:v>5.774468971261975E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.8300000000000004</c:v>
+                  <c:v>5.8194502290712213E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.85000000000000042</c:v>
+                  <c:v>5.8594335693461064E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.87000000000000044</c:v>
+                  <c:v>5.8944189920866308E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.89000000000000046</c:v>
+                  <c:v>5.9244064972927946E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.91000000000000048</c:v>
+                  <c:v>5.9493960849645984E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.93000000000000049</c:v>
+                  <c:v>5.9693877551020409E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.95000000000000051</c:v>
+                  <c:v>5.9843815077051228E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.97000000000000053</c:v>
+                  <c:v>5.9943773427738441E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.99000000000000055</c:v>
+                  <c:v>5.9993752603082047E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.9993752603082047E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.9943773427738441E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.9843815077051228E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.9693877551020409E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.9493960849645984E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.9244064972927953E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.8944189920866315E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.8594335693461071E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.819450229071222E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.7744689712619764E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.7244897959183701E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.6695127030404024E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.6095376926280749E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.5445647646813867E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.4745939192003379E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.3996251561849277E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.3196584756351577E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.2346938775510263E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.1447313619325349E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.049770928779683E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.9498125780924697E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.8448563098708965E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.7349021241149619E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.6199500208246667E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.5000000000000116E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.3750520616409959E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.2451062057476188E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.1101624323198811E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.9702207413577828E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.8252811328613245E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.675343606830505E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.5204081632653247E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.3604748021657846E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.1955435235318838E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.0256143273636221E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.8506872136609993E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.6707621824240153E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.4858392336526713E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.295918367346967E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.1009995835069024E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.9010828821324762E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.69616826322369E-2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.4862557267805429E-2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.2713452728030343E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.0514369012911662E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>8.2653061224493719E-3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.9662640566434727E-3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.6172428154939728E-3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.2182423990008638E-3</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-1.2307371928358534E-3</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-3.7296959600161858E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$50</c:f>
+              <c:f>Sheet1!$A:$A</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="1048576"/>
                 <c:pt idx="0">
-                  <c:v>-9.79575649415021E-4</c:v>
+                  <c:v>1.2500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7164386278009824E-4</c:v>
+                  <c:v>3.7500000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8911362284354601E-3</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.7789014475510582E-3</c:v>
+                  <c:v>8.7499999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6349395201269184E-3</c:v>
+                  <c:v>0.11249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4592504461630021E-3</c:v>
+                  <c:v>0.13749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0251834225659322E-2</c:v>
+                  <c:v>0.16249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.201269085861589E-2</c:v>
+                  <c:v>0.18749999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3741820345032709E-2</c:v>
+                  <c:v>0.21249999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.543922268490977E-2</c:v>
+                  <c:v>0.23749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7104897878247066E-2</c:v>
+                  <c:v>0.26249999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8738845925044607E-2</c:v>
+                  <c:v>0.28749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.0341066825302401E-2</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1911560579020422E-2</c:v>
+                  <c:v>0.33750000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3450327186198688E-2</c:v>
+                  <c:v>0.36250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4957366646837207E-2</c:v>
+                  <c:v>0.38750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6432678960935953E-2</c:v>
+                  <c:v>0.41250000000000009</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.7876264128494942E-2</c:v>
+                  <c:v>0.43750000000000011</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.9288122149514189E-2</c:v>
+                  <c:v>0.46250000000000013</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0668253023993657E-2</c:v>
+                  <c:v>0.48750000000000016</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.2016656751933374E-2</c:v>
+                  <c:v>0.51250000000000018</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.3333333333333347E-2</c:v>
+                  <c:v>0.5375000000000002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.4618282768193544E-2</c:v>
+                  <c:v>0.56250000000000022</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.5871505056513979E-2</c:v>
+                  <c:v>0.58750000000000024</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.709300019829468E-2</c:v>
+                  <c:v>0.61250000000000027</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.8282768193535592E-2</c:v>
+                  <c:v>0.63750000000000029</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.9440809042236777E-2</c:v>
+                  <c:v>0.66250000000000031</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0567122744398179E-2</c:v>
+                  <c:v>0.68750000000000033</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.166170930001984E-2</c:v>
+                  <c:v>0.71250000000000036</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.272456870910174E-2</c:v>
+                  <c:v>0.73750000000000038</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.3755700971643871E-2</c:v>
+                  <c:v>0.7625000000000004</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.4755106087646247E-2</c:v>
+                  <c:v>0.78750000000000042</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.5722784057108869E-2</c:v>
+                  <c:v>0.81250000000000044</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.6658734880031735E-2</c:v>
+                  <c:v>0.83750000000000047</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.7562958556414847E-2</c:v>
+                  <c:v>0.86250000000000049</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.843545508625819E-2</c:v>
+                  <c:v>0.88750000000000051</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.9276224469561779E-2</c:v>
+                  <c:v>0.91250000000000053</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.0085266706325612E-2</c:v>
+                  <c:v>0.93750000000000056</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.0862581796549684E-2</c:v>
+                  <c:v>0.96250000000000058</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.1608169740234001E-2</c:v>
+                  <c:v>0.9875000000000006</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.2322030537378557E-2</c:v>
+                  <c:v>1.0125000000000006</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.3004164187983351E-2</c:v>
+                  <c:v>1.0375000000000005</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.3654570692048396E-2</c:v>
+                  <c:v>1.0625000000000004</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.4273250049573674E-2</c:v>
+                  <c:v>1.0875000000000004</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.4860202260559196E-2</c:v>
+                  <c:v>1.1125000000000003</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.5415427325004971E-2</c:v>
+                  <c:v>1.1375000000000002</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.5938925242910977E-2</c:v>
+                  <c:v>1.1625000000000001</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.6430696014277221E-2</c:v>
+                  <c:v>1.1875</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5.6890739639103717E-2</c:v>
+                  <c:v>1.2124999999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.7319056117390445E-2</c:v>
+                  <c:v>1.2374999999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.2624999999999997</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.2874999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.3124999999999996</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.3374999999999995</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.3624999999999994</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.3874999999999993</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.4124999999999992</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.4374999999999991</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.462499999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.4874999999999989</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.5124999999999988</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.5374999999999988</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.5624999999999987</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5874999999999986</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.6124999999999985</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.6374999999999984</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.6624999999999983</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.6874999999999982</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.7124999999999981</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.737499999999998</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.762499999999998</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.7874999999999979</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.8124999999999978</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.8374999999999977</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.8624999999999976</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.8874999999999975</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.9124999999999974</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.9374999999999973</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.9624999999999972</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.9874999999999972</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.0124999999999971</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.037499999999997</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.0624999999999969</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.0874999999999968</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.1124999999999967</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.1374999999999966</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.1624999999999965</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.1874999999999964</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.2124999999999964</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.2374999999999963</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.2624999999999962</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.2874999999999961</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.312499999999996</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.3374999999999959</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.3624999999999958</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.3874999999999957</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.4124999999999956</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.4374999999999956</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.4624999999999955</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.4874999999999954</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.5124999999999953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,7 +862,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -596,7 +924,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1536,10 +1864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:Y104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1547,543 +1875,1668 @@
     <col min="2" max="2" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2">
-        <f>$D$1+($F$1/2)</f>
-        <v>0.01</v>
+        <f>$W$1+($Y$1/2)</f>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="B1" s="3">
-        <f>$F$2*(1-( (A1-$D$3) / $D$4)^2)</f>
-        <v>-9.79575649415021E-4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+        <f>$Y$2*(1-( (A1-$W$3) / $W$4)^2)</f>
+        <v>-1.2307371928363064E-3</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2">
+        <v>0</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="4">
+        <v>0</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="Y1" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <f>A1+$F$1</f>
-        <v>0.03</v>
+        <f>A1+$Y$1</f>
+        <v>3.7500000000000006E-2</v>
       </c>
       <c r="B2" s="3">
-        <f t="shared" ref="B2:B50" si="0">$F$2*(1-( (A2-$D$3) / $D$4)^2)</f>
-        <v>9.7164386278009824E-4</v>
-      </c>
-      <c r="C2" t="s">
+        <f>$Y$2*(1-( (A2-$W$3) / $W$4)^2)</f>
+        <v>1.218242399000431E-3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="W2" s="4">
         <v>2.5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="X2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="Y2" s="4">
         <v>0.06</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <f t="shared" ref="A3:A50" si="1">A2+$F$1</f>
-        <v>0.05</v>
+        <f>A2+$Y$1</f>
+        <v>6.25E-2</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" si="0"/>
-        <v>2.8911362284354601E-3</v>
-      </c>
-      <c r="C3" t="s">
+        <f>$Y$2*(1-( (A3-$W$3) / $W$4)^2)</f>
+        <v>3.6172428154935465E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <f>$D$1 + (($D$2-$D$1)/2)</f>
+      <c r="W3">
+        <f>$W$1 + (($W$2-$W$1)/2)</f>
         <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <f>A3+$Y$1</f>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" si="0"/>
-        <v>4.7789014475510582E-3</v>
-      </c>
-      <c r="C4" t="s">
+        <f>$Y$2*(1-( (A4-$W$3) / $W$4)^2)</f>
+        <v>5.9662640566430598E-3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="V4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
-        <f>($F$1)-(($D$2-$D$1)/2)</f>
-        <v>-1.23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="W4" s="1">
+        <f>($Y$1)-(($W$2-$W$1)/2)</f>
+        <v>-1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <f t="shared" si="1"/>
-        <v>9.0000000000000011E-2</v>
+        <f>A4+$Y$1</f>
+        <v>0.11249999999999999</v>
       </c>
       <c r="B5" s="3">
-        <f t="shared" si="0"/>
-        <v>6.6349395201269184E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A5-$W$3) / $W$4)^2)</f>
+        <v>8.265306122448985E-3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11000000000000001</v>
+        <f>A5+$Y$1</f>
+        <v>0.13749999999999998</v>
       </c>
       <c r="B6" s="3">
-        <f t="shared" si="0"/>
-        <v>8.4592504461630021E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A6-$W$3) / $W$4)^2)</f>
+        <v>1.0514369012911289E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.13</v>
+        <f>A6+$Y$1</f>
+        <v>0.16249999999999998</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" si="0"/>
-        <v>1.0251834225659322E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A7-$W$3) / $W$4)^2)</f>
+        <v>1.2713452728030003E-2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
-        <v>0.15</v>
+        <f>A7+$Y$1</f>
+        <v>0.18749999999999997</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.201269085861589E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A8-$W$3) / $W$4)^2)</f>
+        <v>1.4862557267805082E-2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
-        <v>0.16999999999999998</v>
+        <f>A8+$Y$1</f>
+        <v>0.21249999999999997</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" si="0"/>
-        <v>1.3741820345032709E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A9-$W$3) / $W$4)^2)</f>
+        <v>1.696168263223656E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
-        <v>0.18999999999999997</v>
+        <f>A9+$Y$1</f>
+        <v>0.23749999999999996</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" si="0"/>
-        <v>1.543922268490977E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A10-$W$3) / $W$4)^2)</f>
+        <v>1.9010828821324457E-2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.20999999999999996</v>
+        <f>A10+$Y$1</f>
+        <v>0.26249999999999996</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" si="0"/>
-        <v>1.7104897878247066E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A11-$W$3) / $W$4)^2)</f>
+        <v>2.1009995835068716E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.22999999999999995</v>
+        <f>A11+$Y$1</f>
+        <v>0.28749999999999998</v>
       </c>
       <c r="B12" s="3">
-        <f t="shared" si="0"/>
-        <v>1.8738845925044607E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A12-$W$3) / $W$4)^2)</f>
+        <v>2.2959183673469389E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.24999999999999994</v>
+        <f>A12+$Y$1</f>
+        <v>0.3125</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>2.0341066825302401E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A13-$W$3) / $W$4)^2)</f>
+        <v>2.4858392336526453E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <f t="shared" si="1"/>
-        <v>0.26999999999999996</v>
+        <f>A13+$Y$1</f>
+        <v>0.33750000000000002</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>2.1911560579020422E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A14-$W$3) / $W$4)^2)</f>
+        <v>2.6707621824239906E-2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <f t="shared" si="1"/>
-        <v>0.28999999999999998</v>
+        <f>A14+$Y$1</f>
+        <v>0.36250000000000004</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3450327186198688E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A15-$W$3) / $W$4)^2)</f>
+        <v>2.8506872136609754E-2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31</v>
+        <f>A15+$Y$1</f>
+        <v>0.38750000000000007</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>2.4957366646837207E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A16-$W$3) / $W$4)^2)</f>
+        <v>3.0256143273635992E-2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <f t="shared" si="1"/>
-        <v>0.33</v>
+        <f>A16+$Y$1</f>
+        <v>0.41250000000000009</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>2.6432678960935953E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A17-$W$3) / $W$4)^2)</f>
+        <v>3.195543523531863E-2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <f t="shared" si="1"/>
-        <v>0.35000000000000003</v>
+        <f>A17+$Y$1</f>
+        <v>0.43750000000000011</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>2.7876264128494942E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A18-$W$3) / $W$4)^2)</f>
+        <v>3.3604748021657659E-2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <f t="shared" si="1"/>
-        <v>0.37000000000000005</v>
+        <f>A18+$Y$1</f>
+        <v>0.46250000000000013</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>2.9288122149514189E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A19-$W$3) / $W$4)^2)</f>
+        <v>3.5204081632653074E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.39000000000000007</v>
+        <f>A19+$Y$1</f>
+        <v>0.48750000000000016</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>3.0668253023993657E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A20-$W$3) / $W$4)^2)</f>
+        <v>3.6753436068304883E-2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.41000000000000009</v>
+        <f>A20+$Y$1</f>
+        <v>0.51250000000000018</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>3.2016656751933374E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A21-$W$3) / $W$4)^2)</f>
+        <v>3.8252811328613086E-2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <f t="shared" si="1"/>
-        <v>0.4300000000000001</v>
+        <f>A21+$Y$1</f>
+        <v>0.5375000000000002</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>3.3333333333333347E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A22-$W$3) / $W$4)^2)</f>
+        <v>3.9702207413577696E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <f t="shared" si="1"/>
-        <v>0.45000000000000012</v>
+        <f>A22+$Y$1</f>
+        <v>0.56250000000000022</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>3.4618282768193544E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A23-$W$3) / $W$4)^2)</f>
+        <v>4.1101624323198679E-2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <f t="shared" si="1"/>
-        <v>0.47000000000000014</v>
+        <f>A23+$Y$1</f>
+        <v>0.58750000000000024</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>3.5871505056513979E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A24-$W$3) / $W$4)^2)</f>
+        <v>4.245106205747607E-2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <f t="shared" si="1"/>
-        <v>0.49000000000000016</v>
+        <f>A24+$Y$1</f>
+        <v>0.61250000000000027</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="0"/>
-        <v>3.709300019829468E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A25-$W$3) / $W$4)^2)</f>
+        <v>4.3750520616409848E-2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <f t="shared" si="1"/>
-        <v>0.51000000000000012</v>
+        <f>A25+$Y$1</f>
+        <v>0.63750000000000029</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="0"/>
-        <v>3.8282768193535592E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A26-$W$3) / $W$4)^2)</f>
+        <v>4.5000000000000012E-2</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <f t="shared" si="1"/>
-        <v>0.53000000000000014</v>
+        <f>A26+$Y$1</f>
+        <v>0.66250000000000031</v>
       </c>
       <c r="B27" s="3">
-        <f t="shared" si="0"/>
-        <v>3.9440809042236777E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A27-$W$3) / $W$4)^2)</f>
+        <v>4.6199500208246577E-2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
-        <v>0.55000000000000016</v>
+        <f>A27+$Y$1</f>
+        <v>0.68750000000000033</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" si="0"/>
-        <v>4.0567122744398179E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A28-$W$3) / $W$4)^2)</f>
+        <v>4.7349021241149536E-2</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
-        <v>0.57000000000000017</v>
+        <f>A28+$Y$1</f>
+        <v>0.71250000000000036</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" si="0"/>
-        <v>4.166170930001984E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A29-$W$3) / $W$4)^2)</f>
+        <v>4.8448563098708888E-2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <f t="shared" si="1"/>
-        <v>0.59000000000000019</v>
+        <f>A29+$Y$1</f>
+        <v>0.73750000000000038</v>
       </c>
       <c r="B30" s="3">
-        <f t="shared" si="0"/>
-        <v>4.272456870910174E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A30-$W$3) / $W$4)^2)</f>
+        <v>4.9498125780924634E-2</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <f t="shared" si="1"/>
-        <v>0.61000000000000021</v>
+        <f>A30+$Y$1</f>
+        <v>0.7625000000000004</v>
       </c>
       <c r="B31" s="3">
-        <f t="shared" si="0"/>
-        <v>4.3755700971643871E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A31-$W$3) / $W$4)^2)</f>
+        <v>5.049770928779676E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <f t="shared" si="1"/>
-        <v>0.63000000000000023</v>
+        <f>A31+$Y$1</f>
+        <v>0.78750000000000042</v>
       </c>
       <c r="B32" s="3">
-        <f t="shared" si="0"/>
-        <v>4.4755106087646247E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A32-$W$3) / $W$4)^2)</f>
+        <v>5.1447313619325294E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <f t="shared" si="1"/>
-        <v>0.65000000000000024</v>
+        <f>A32+$Y$1</f>
+        <v>0.81250000000000044</v>
       </c>
       <c r="B33" s="3">
-        <f t="shared" si="0"/>
-        <v>4.5722784057108869E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A33-$W$3) / $W$4)^2)</f>
+        <v>5.2346938775510214E-2</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <f t="shared" si="1"/>
-        <v>0.67000000000000026</v>
+        <f>A33+$Y$1</f>
+        <v>0.83750000000000047</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" si="0"/>
-        <v>4.6658734880031735E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A34-$W$3) / $W$4)^2)</f>
+        <v>5.3196584756351535E-2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <f t="shared" si="1"/>
-        <v>0.69000000000000028</v>
+        <f>A34+$Y$1</f>
+        <v>0.86250000000000049</v>
       </c>
       <c r="B35" s="3">
-        <f t="shared" si="0"/>
-        <v>4.7562958556414847E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A35-$W$3) / $W$4)^2)</f>
+        <v>5.3996251561849243E-2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <f t="shared" si="1"/>
-        <v>0.7100000000000003</v>
+        <f>A35+$Y$1</f>
+        <v>0.88750000000000051</v>
       </c>
       <c r="B36" s="3">
-        <f t="shared" si="0"/>
-        <v>4.843545508625819E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A36-$W$3) / $W$4)^2)</f>
+        <v>5.4745939192003344E-2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <f t="shared" si="1"/>
-        <v>0.73000000000000032</v>
+        <f>A36+$Y$1</f>
+        <v>0.91250000000000053</v>
       </c>
       <c r="B37" s="3">
-        <f t="shared" si="0"/>
-        <v>4.9276224469561779E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A37-$W$3) / $W$4)^2)</f>
+        <v>5.5445647646813839E-2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <f t="shared" si="1"/>
-        <v>0.75000000000000033</v>
+        <f>A37+$Y$1</f>
+        <v>0.93750000000000056</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" si="0"/>
-        <v>5.0085266706325612E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A38-$W$3) / $W$4)^2)</f>
+        <v>5.6095376926280728E-2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <f t="shared" si="1"/>
-        <v>0.77000000000000035</v>
+        <f>A38+$Y$1</f>
+        <v>0.96250000000000058</v>
       </c>
       <c r="B39" s="3">
-        <f t="shared" si="0"/>
-        <v>5.0862581796549684E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A39-$W$3) / $W$4)^2)</f>
+        <v>5.6695127030404011E-2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <f t="shared" si="1"/>
-        <v>0.79000000000000037</v>
+        <f>A39+$Y$1</f>
+        <v>0.9875000000000006</v>
       </c>
       <c r="B40" s="3">
-        <f t="shared" si="0"/>
-        <v>5.1608169740234001E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A40-$W$3) / $W$4)^2)</f>
+        <v>5.7244897959183687E-2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <f t="shared" si="1"/>
-        <v>0.81000000000000039</v>
+        <f>A40+$Y$1</f>
+        <v>1.0125000000000006</v>
       </c>
       <c r="B41" s="3">
-        <f t="shared" si="0"/>
-        <v>5.2322030537378557E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A41-$W$3) / $W$4)^2)</f>
+        <v>5.774468971261975E-2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <f t="shared" si="1"/>
-        <v>0.8300000000000004</v>
+        <f>A41+$Y$1</f>
+        <v>1.0375000000000005</v>
       </c>
       <c r="B42" s="3">
-        <f t="shared" si="0"/>
-        <v>5.3004164187983351E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A42-$W$3) / $W$4)^2)</f>
+        <v>5.8194502290712213E-2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <f t="shared" si="1"/>
-        <v>0.85000000000000042</v>
+        <f>A42+$Y$1</f>
+        <v>1.0625000000000004</v>
       </c>
       <c r="B43" s="3">
-        <f t="shared" si="0"/>
-        <v>5.3654570692048396E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A43-$W$3) / $W$4)^2)</f>
+        <v>5.8594335693461064E-2</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <f t="shared" si="1"/>
-        <v>0.87000000000000044</v>
+        <f>A43+$Y$1</f>
+        <v>1.0875000000000004</v>
       </c>
       <c r="B44" s="3">
-        <f t="shared" si="0"/>
-        <v>5.4273250049573674E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A44-$W$3) / $W$4)^2)</f>
+        <v>5.8944189920866308E-2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <f t="shared" si="1"/>
-        <v>0.89000000000000046</v>
+        <f>A44+$Y$1</f>
+        <v>1.1125000000000003</v>
       </c>
       <c r="B45" s="3">
-        <f t="shared" si="0"/>
-        <v>5.4860202260559196E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A45-$W$3) / $W$4)^2)</f>
+        <v>5.9244064972927946E-2</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <f t="shared" si="1"/>
-        <v>0.91000000000000048</v>
+        <f>A45+$Y$1</f>
+        <v>1.1375000000000002</v>
       </c>
       <c r="B46" s="3">
-        <f t="shared" si="0"/>
-        <v>5.5415427325004971E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A46-$W$3) / $W$4)^2)</f>
+        <v>5.9493960849645984E-2</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <f t="shared" si="1"/>
-        <v>0.93000000000000049</v>
+        <f>A46+$Y$1</f>
+        <v>1.1625000000000001</v>
       </c>
       <c r="B47" s="3">
-        <f t="shared" si="0"/>
-        <v>5.5938925242910977E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A47-$W$3) / $W$4)^2)</f>
+        <v>5.9693877551020409E-2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <f t="shared" si="1"/>
-        <v>0.95000000000000051</v>
+        <f>A47+$Y$1</f>
+        <v>1.1875</v>
       </c>
       <c r="B48" s="3">
-        <f t="shared" si="0"/>
-        <v>5.6430696014277221E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A48-$W$3) / $W$4)^2)</f>
+        <v>5.9843815077051228E-2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <f t="shared" si="1"/>
-        <v>0.97000000000000053</v>
+        <f>A48+$Y$1</f>
+        <v>1.2124999999999999</v>
       </c>
       <c r="B49" s="3">
-        <f t="shared" si="0"/>
-        <v>5.6890739639103717E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+        <f>$Y$2*(1-( (A49-$W$3) / $W$4)^2)</f>
+        <v>5.9943773427738441E-2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <f t="shared" si="1"/>
-        <v>0.99000000000000055</v>
+        <f>A49+$Y$1</f>
+        <v>1.2374999999999998</v>
       </c>
       <c r="B50" s="3">
-        <f t="shared" si="0"/>
-        <v>5.7319056117390445E-2</v>
-      </c>
+        <f>$Y$2*(1-( (A50-$W$3) / $W$4)^2)</f>
+        <v>5.9993752603082047E-2</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <f>A50+$Y$1</f>
+        <v>1.2624999999999997</v>
+      </c>
+      <c r="B51" s="3">
+        <f>$Y$2*(1-( (A51-$W$3) / $W$4)^2)</f>
+        <v>5.9993752603082047E-2</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <f>A51+$Y$1</f>
+        <v>1.2874999999999996</v>
+      </c>
+      <c r="B52" s="3">
+        <f>$Y$2*(1-( (A52-$W$3) / $W$4)^2)</f>
+        <v>5.9943773427738441E-2</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <f>A52+$Y$1</f>
+        <v>1.3124999999999996</v>
+      </c>
+      <c r="B53" s="3">
+        <f>$Y$2*(1-( (A53-$W$3) / $W$4)^2)</f>
+        <v>5.9843815077051228E-2</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <f>A53+$Y$1</f>
+        <v>1.3374999999999995</v>
+      </c>
+      <c r="B54" s="3">
+        <f>$Y$2*(1-( (A54-$W$3) / $W$4)^2)</f>
+        <v>5.9693877551020409E-2</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <f>A54+$Y$1</f>
+        <v>1.3624999999999994</v>
+      </c>
+      <c r="B55" s="3">
+        <f>$Y$2*(1-( (A55-$W$3) / $W$4)^2)</f>
+        <v>5.9493960849645984E-2</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <f>A55+$Y$1</f>
+        <v>1.3874999999999993</v>
+      </c>
+      <c r="B56" s="3">
+        <f>$Y$2*(1-( (A56-$W$3) / $W$4)^2)</f>
+        <v>5.9244064972927953E-2</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <f>A56+$Y$1</f>
+        <v>1.4124999999999992</v>
+      </c>
+      <c r="B57" s="3">
+        <f>$Y$2*(1-( (A57-$W$3) / $W$4)^2)</f>
+        <v>5.8944189920866315E-2</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <f>A57+$Y$1</f>
+        <v>1.4374999999999991</v>
+      </c>
+      <c r="B58" s="3">
+        <f>$Y$2*(1-( (A58-$W$3) / $W$4)^2)</f>
+        <v>5.8594335693461071E-2</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <f>A58+$Y$1</f>
+        <v>1.462499999999999</v>
+      </c>
+      <c r="B59" s="3">
+        <f>$Y$2*(1-( (A59-$W$3) / $W$4)^2)</f>
+        <v>5.819450229071222E-2</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <f>A59+$Y$1</f>
+        <v>1.4874999999999989</v>
+      </c>
+      <c r="B60" s="3">
+        <f>$Y$2*(1-( (A60-$W$3) / $W$4)^2)</f>
+        <v>5.7744689712619764E-2</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <f>A60+$Y$1</f>
+        <v>1.5124999999999988</v>
+      </c>
+      <c r="B61" s="3">
+        <f>$Y$2*(1-( (A61-$W$3) / $W$4)^2)</f>
+        <v>5.7244897959183701E-2</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <f>A61+$Y$1</f>
+        <v>1.5374999999999988</v>
+      </c>
+      <c r="B62" s="3">
+        <f>$Y$2*(1-( (A62-$W$3) / $W$4)^2)</f>
+        <v>5.6695127030404024E-2</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <f>A62+$Y$1</f>
+        <v>1.5624999999999987</v>
+      </c>
+      <c r="B63" s="3">
+        <f>$Y$2*(1-( (A63-$W$3) / $W$4)^2)</f>
+        <v>5.6095376926280749E-2</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <f>A63+$Y$1</f>
+        <v>1.5874999999999986</v>
+      </c>
+      <c r="B64" s="3">
+        <f>$Y$2*(1-( (A64-$W$3) / $W$4)^2)</f>
+        <v>5.5445647646813867E-2</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <f>A64+$Y$1</f>
+        <v>1.6124999999999985</v>
+      </c>
+      <c r="B65" s="3">
+        <f>$Y$2*(1-( (A65-$W$3) / $W$4)^2)</f>
+        <v>5.4745939192003379E-2</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <f>A65+$Y$1</f>
+        <v>1.6374999999999984</v>
+      </c>
+      <c r="B66" s="3">
+        <f>$Y$2*(1-( (A66-$W$3) / $W$4)^2)</f>
+        <v>5.3996251561849277E-2</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <f>A66+$Y$1</f>
+        <v>1.6624999999999983</v>
+      </c>
+      <c r="B67" s="3">
+        <f>$Y$2*(1-( (A67-$W$3) / $W$4)^2)</f>
+        <v>5.3196584756351577E-2</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <f>A67+$Y$1</f>
+        <v>1.6874999999999982</v>
+      </c>
+      <c r="B68" s="3">
+        <f>$Y$2*(1-( (A68-$W$3) / $W$4)^2)</f>
+        <v>5.2346938775510263E-2</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <f>A68+$Y$1</f>
+        <v>1.7124999999999981</v>
+      </c>
+      <c r="B69" s="3">
+        <f>$Y$2*(1-( (A69-$W$3) / $W$4)^2)</f>
+        <v>5.1447313619325349E-2</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <f>A69+$Y$1</f>
+        <v>1.737499999999998</v>
+      </c>
+      <c r="B70" s="3">
+        <f>$Y$2*(1-( (A70-$W$3) / $W$4)^2)</f>
+        <v>5.049770928779683E-2</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <f>A70+$Y$1</f>
+        <v>1.762499999999998</v>
+      </c>
+      <c r="B71" s="3">
+        <f>$Y$2*(1-( (A71-$W$3) / $W$4)^2)</f>
+        <v>4.9498125780924697E-2</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <f>A71+$Y$1</f>
+        <v>1.7874999999999979</v>
+      </c>
+      <c r="B72" s="3">
+        <f>$Y$2*(1-( (A72-$W$3) / $W$4)^2)</f>
+        <v>4.8448563098708965E-2</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <f>A72+$Y$1</f>
+        <v>1.8124999999999978</v>
+      </c>
+      <c r="B73" s="3">
+        <f>$Y$2*(1-( (A73-$W$3) / $W$4)^2)</f>
+        <v>4.7349021241149619E-2</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <f>A73+$Y$1</f>
+        <v>1.8374999999999977</v>
+      </c>
+      <c r="B74" s="3">
+        <f>$Y$2*(1-( (A74-$W$3) / $W$4)^2)</f>
+        <v>4.6199500208246667E-2</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <f>A74+$Y$1</f>
+        <v>1.8624999999999976</v>
+      </c>
+      <c r="B75" s="3">
+        <f>$Y$2*(1-( (A75-$W$3) / $W$4)^2)</f>
+        <v>4.5000000000000116E-2</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <f>A75+$Y$1</f>
+        <v>1.8874999999999975</v>
+      </c>
+      <c r="B76" s="3">
+        <f>$Y$2*(1-( (A76-$W$3) / $W$4)^2)</f>
+        <v>4.3750520616409959E-2</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <f>A76+$Y$1</f>
+        <v>1.9124999999999974</v>
+      </c>
+      <c r="B77" s="3">
+        <f>$Y$2*(1-( (A77-$W$3) / $W$4)^2)</f>
+        <v>4.2451062057476188E-2</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <f>A77+$Y$1</f>
+        <v>1.9374999999999973</v>
+      </c>
+      <c r="B78" s="3">
+        <f>$Y$2*(1-( (A78-$W$3) / $W$4)^2)</f>
+        <v>4.1101624323198811E-2</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
+        <f>A78+$Y$1</f>
+        <v>1.9624999999999972</v>
+      </c>
+      <c r="B79" s="3">
+        <f>$Y$2*(1-( (A79-$W$3) / $W$4)^2)</f>
+        <v>3.9702207413577828E-2</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <f>A79+$Y$1</f>
+        <v>1.9874999999999972</v>
+      </c>
+      <c r="B80" s="3">
+        <f>$Y$2*(1-( (A80-$W$3) / $W$4)^2)</f>
+        <v>3.8252811328613245E-2</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <f>A80+$Y$1</f>
+        <v>2.0124999999999971</v>
+      </c>
+      <c r="B81" s="3">
+        <f>$Y$2*(1-( (A81-$W$3) / $W$4)^2)</f>
+        <v>3.675343606830505E-2</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <f>A81+$Y$1</f>
+        <v>2.037499999999997</v>
+      </c>
+      <c r="B82" s="3">
+        <f>$Y$2*(1-( (A82-$W$3) / $W$4)^2)</f>
+        <v>3.5204081632653247E-2</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0</v>
+      </c>
+      <c r="D82" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <f>A82+$Y$1</f>
+        <v>2.0624999999999969</v>
+      </c>
+      <c r="B83" s="3">
+        <f>$Y$2*(1-( (A83-$W$3) / $W$4)^2)</f>
+        <v>3.3604748021657846E-2</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <f>A83+$Y$1</f>
+        <v>2.0874999999999968</v>
+      </c>
+      <c r="B84" s="3">
+        <f>$Y$2*(1-( (A84-$W$3) / $W$4)^2)</f>
+        <v>3.1955435235318838E-2</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <f>A84+$Y$1</f>
+        <v>2.1124999999999967</v>
+      </c>
+      <c r="B85" s="3">
+        <f>$Y$2*(1-( (A85-$W$3) / $W$4)^2)</f>
+        <v>3.0256143273636221E-2</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
+        <f>A85+$Y$1</f>
+        <v>2.1374999999999966</v>
+      </c>
+      <c r="B86" s="3">
+        <f>$Y$2*(1-( (A86-$W$3) / $W$4)^2)</f>
+        <v>2.8506872136609993E-2</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <f>A86+$Y$1</f>
+        <v>2.1624999999999965</v>
+      </c>
+      <c r="B87" s="3">
+        <f>$Y$2*(1-( (A87-$W$3) / $W$4)^2)</f>
+        <v>2.6707621824240153E-2</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <f>A87+$Y$1</f>
+        <v>2.1874999999999964</v>
+      </c>
+      <c r="B88" s="3">
+        <f>$Y$2*(1-( (A88-$W$3) / $W$4)^2)</f>
+        <v>2.4858392336526713E-2</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0</v>
+      </c>
+      <c r="D88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <f>A88+$Y$1</f>
+        <v>2.2124999999999964</v>
+      </c>
+      <c r="B89" s="3">
+        <f>$Y$2*(1-( (A89-$W$3) / $W$4)^2)</f>
+        <v>2.295918367346967E-2</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <f>A89+$Y$1</f>
+        <v>2.2374999999999963</v>
+      </c>
+      <c r="B90" s="3">
+        <f>$Y$2*(1-( (A90-$W$3) / $W$4)^2)</f>
+        <v>2.1009995835069024E-2</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="2">
+        <f>A90+$Y$1</f>
+        <v>2.2624999999999962</v>
+      </c>
+      <c r="B91" s="3">
+        <f>$Y$2*(1-( (A91-$W$3) / $W$4)^2)</f>
+        <v>1.9010828821324762E-2</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <f>A91+$Y$1</f>
+        <v>2.2874999999999961</v>
+      </c>
+      <c r="B92" s="3">
+        <f>$Y$2*(1-( (A92-$W$3) / $W$4)^2)</f>
+        <v>1.69616826322369E-2</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
+        <f>A92+$Y$1</f>
+        <v>2.312499999999996</v>
+      </c>
+      <c r="B93" s="3">
+        <f>$Y$2*(1-( (A93-$W$3) / $W$4)^2)</f>
+        <v>1.4862557267805429E-2</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <f>A93+$Y$1</f>
+        <v>2.3374999999999959</v>
+      </c>
+      <c r="B94" s="3">
+        <f>$Y$2*(1-( (A94-$W$3) / $W$4)^2)</f>
+        <v>1.2713452728030343E-2</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <f>A94+$Y$1</f>
+        <v>2.3624999999999958</v>
+      </c>
+      <c r="B95" s="3">
+        <f>$Y$2*(1-( (A95-$W$3) / $W$4)^2)</f>
+        <v>1.0514369012911662E-2</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <f>A95+$Y$1</f>
+        <v>2.3874999999999957</v>
+      </c>
+      <c r="B96" s="3">
+        <f>$Y$2*(1-( (A96-$W$3) / $W$4)^2)</f>
+        <v>8.2653061224493719E-3</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <f>A96+$Y$1</f>
+        <v>2.4124999999999956</v>
+      </c>
+      <c r="B97" s="3">
+        <f>$Y$2*(1-( (A97-$W$3) / $W$4)^2)</f>
+        <v>5.9662640566434727E-3</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <f>A97+$Y$1</f>
+        <v>2.4374999999999956</v>
+      </c>
+      <c r="B98" s="3">
+        <f>$Y$2*(1-( (A98-$W$3) / $W$4)^2)</f>
+        <v>3.6172428154939728E-3</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <f>A98+$Y$1</f>
+        <v>2.4624999999999955</v>
+      </c>
+      <c r="B99" s="3">
+        <f>$Y$2*(1-( (A99-$W$3) / $W$4)^2)</f>
+        <v>1.2182423990008638E-3</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <f>A99+$Y$1</f>
+        <v>2.4874999999999954</v>
+      </c>
+      <c r="B100" s="3">
+        <f>$Y$2*(1-( (A100-$W$3) / $W$4)^2)</f>
+        <v>-1.2307371928358534E-3</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <f>A100+$Y$1</f>
+        <v>2.5124999999999953</v>
+      </c>
+      <c r="B101" s="3">
+        <f>$Y$2*(1-( (A101-$W$3) / $W$4)^2)</f>
+        <v>-3.7296959600161858E-3</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>